<commit_message>
Aba Investimentos - Projeto
</commit_message>
<xml_diff>
--- a/Projeto/Projeto - Controle Mercado.xlsx
+++ b/Projeto/Projeto - Controle Mercado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAN\Desktop\Curso-Excel\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CA68A3-FAF9-4088-A7A9-5C4D0445483F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E062A86A-E8F5-4662-BD18-F42F9B17FBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
   <si>
     <t>Resultados</t>
   </si>
@@ -323,6 +323,27 @@
   </si>
   <si>
     <t>Total de Despesas</t>
+  </si>
+  <si>
+    <t>Investimento</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Estrutura</t>
+  </si>
+  <si>
+    <t>Outras</t>
+  </si>
+  <si>
+    <t>Equipamentos (Carrinhos, Balanças, Cortador de Queijo, etc)</t>
+  </si>
+  <si>
+    <t>Documentação, Sistema de Informação, Estrutura Inicial, Sistema de Refrigeração, Equipamentos</t>
   </si>
 </sst>
 </file>
@@ -423,7 +444,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -442,21 +463,34 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -923,20 +957,33 @@
     <sortCondition descending="1" ref="B4:B26"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{70F01BB3-039F-4F6A-9127-0FE396F11917}" name="Data" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{70F01BB3-039F-4F6A-9127-0FE396F11917}" name="Data" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{23FDBB76-891B-4BEF-88E5-CF45534E4FA6}" name="Fornecedor"/>
     <tableColumn id="3" xr3:uid="{47E77675-1CB5-4223-999C-CD7D30DA4298}" name="Mercadoria"/>
-    <tableColumn id="4" xr3:uid="{50509D53-9FDE-434A-A21C-765E6322AE8A}" name="Medida" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{50509D53-9FDE-434A-A21C-765E6322AE8A}" name="Medida" dataDxfId="5">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela2[[#This Row],[Mercadoria]],cálculos!$M$7:$P$34,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{FF08DCA9-D260-4B65-9D79-32D0EDA3AD9A}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{BDD50E25-5158-4F1F-BC90-ABBF12938393}" name="Preço Unitário" dataDxfId="0" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{BDD50E25-5158-4F1F-BC90-ABBF12938393}" name="Preço Unitário" dataDxfId="4" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela2[[#This Row],[Mercadoria]],cálculos!$M$7:$P$34,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{FBF94F4E-37BE-4D76-BDDD-D3C765A36413}" name="Desconto" dataCellStyle="Porcentagem"/>
-    <tableColumn id="8" xr3:uid="{AEFD3C74-15EE-4D2B-9559-6E09557523AE}" name="Valor Pago" dataDxfId="2" dataCellStyle="Moeda">
+    <tableColumn id="8" xr3:uid="{AEFD3C74-15EE-4D2B-9559-6E09557523AE}" name="Valor Pago" dataDxfId="3" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4260D52-81F2-4162-98BF-30718AC2EAF3}" name="Tabela4" displayName="Tabela4" ref="B4:E9" totalsRowShown="0">
+  <autoFilter ref="B4:E9" xr:uid="{C4260D52-81F2-4162-98BF-30718AC2EAF3}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3DE2EC2D-FE65-43D5-9E03-63CA32193761}" name="Investimento" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{129E839C-F6BB-4D91-906F-D4AE5BA48C18}" name="Data" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{81A341C0-EC03-4544-8A0B-6ECB312FEAC6}" name="Descrição" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{8DA02AF3-1548-4A14-9A42-6E5373D624E7}" name="Valor" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1253,9 +1300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1576,9 +1621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:I28"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2245,13 +2288,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="14">
+        <v>43590</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="4">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B11" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13">
+        <f>SUM(Tabela4[Valor])</f>
+        <v>400000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aba Controle de Estoque - Projeto
</commit_message>
<xml_diff>
--- a/Projeto/Projeto - Controle Mercado.xlsx
+++ b/Projeto/Projeto - Controle Mercado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAN\Desktop\Curso-Excel\Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zero\Desktop\Curso-Excel\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E062A86A-E8F5-4662-BD18-F42F9B17FBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7108EB-18A7-467E-86F2-1AD9E26118A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,26 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">cálculos!$M$6:$P$6</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="110">
   <si>
     <t>Resultados</t>
   </si>
@@ -344,17 +353,39 @@
   </si>
   <si>
     <t>Documentação, Sistema de Informação, Estrutura Inicial, Sistema de Refrigeração, Equipamentos</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Data da Última Compra</t>
+  </si>
+  <si>
+    <t>Quantidade Inicial</t>
+  </si>
+  <si>
+    <t>Quantidade Comprada</t>
+  </si>
+  <si>
+    <t>Quantidade Vendida</t>
+  </si>
+  <si>
+    <t>Quantidade Atual</t>
+  </si>
+  <si>
+    <t>Situação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,8 +424,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +443,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,12 +484,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -467,13 +513,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+    <cellStyle name="Moeda 2" xfId="3" xr:uid="{43C612B4-AE4A-476B-8C1F-D416BCD9B058}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -498,6 +648,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -957,18 +1113,18 @@
     <sortCondition descending="1" ref="B4:B26"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{70F01BB3-039F-4F6A-9127-0FE396F11917}" name="Data" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{70F01BB3-039F-4F6A-9127-0FE396F11917}" name="Data" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{23FDBB76-891B-4BEF-88E5-CF45534E4FA6}" name="Fornecedor"/>
     <tableColumn id="3" xr3:uid="{47E77675-1CB5-4223-999C-CD7D30DA4298}" name="Mercadoria"/>
-    <tableColumn id="4" xr3:uid="{50509D53-9FDE-434A-A21C-765E6322AE8A}" name="Medida" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{50509D53-9FDE-434A-A21C-765E6322AE8A}" name="Medida" dataDxfId="21">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela2[[#This Row],[Mercadoria]],cálculos!$M$7:$P$34,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{FF08DCA9-D260-4B65-9D79-32D0EDA3AD9A}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{BDD50E25-5158-4F1F-BC90-ABBF12938393}" name="Preço Unitário" dataDxfId="4" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{BDD50E25-5158-4F1F-BC90-ABBF12938393}" name="Preço Unitário" dataDxfId="20" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela2[[#This Row],[Mercadoria]],cálculos!$M$7:$P$34,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{FBF94F4E-37BE-4D76-BDDD-D3C765A36413}" name="Desconto" dataCellStyle="Porcentagem"/>
-    <tableColumn id="8" xr3:uid="{AEFD3C74-15EE-4D2B-9559-6E09557523AE}" name="Valor Pago" dataDxfId="3" dataCellStyle="Moeda">
+    <tableColumn id="8" xr3:uid="{AEFD3C74-15EE-4D2B-9559-6E09557523AE}" name="Valor Pago" dataDxfId="19" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -980,12 +1136,34 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4260D52-81F2-4162-98BF-30718AC2EAF3}" name="Tabela4" displayName="Tabela4" ref="B4:E9" totalsRowShown="0">
   <autoFilter ref="B4:E9" xr:uid="{C4260D52-81F2-4162-98BF-30718AC2EAF3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3DE2EC2D-FE65-43D5-9E03-63CA32193761}" name="Investimento" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{129E839C-F6BB-4D91-906F-D4AE5BA48C18}" name="Data" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{81A341C0-EC03-4544-8A0B-6ECB312FEAC6}" name="Descrição" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3DE2EC2D-FE65-43D5-9E03-63CA32193761}" name="Investimento" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{129E839C-F6BB-4D91-906F-D4AE5BA48C18}" name="Data" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{81A341C0-EC03-4544-8A0B-6ECB312FEAC6}" name="Descrição" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{8DA02AF3-1548-4A14-9A42-6E5373D624E7}" name="Valor" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64CF6E44-08DA-45E7-A768-DF394F8148AD}" name="Tabela1" displayName="Tabela1" ref="B4:H28">
+  <autoFilter ref="B4:H28" xr:uid="{64CF6E44-08DA-45E7-A768-DF394F8148AD}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{46C366B8-BE15-4500-9E9A-C4C93EDADFBF}" name="Produto" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{9D624FE4-2073-40B5-AD69-FB6399F49BF6}" name="Data da Última Compra"/>
+    <tableColumn id="3" xr3:uid="{34D575FB-E869-42B1-9733-C1CFD882C0FC}" name="Quantidade Inicial"/>
+    <tableColumn id="4" xr3:uid="{28E8EF48-C2E8-4765-B5A6-39213CF6B625}" name="Quantidade Comprada" dataDxfId="15">
+      <calculatedColumnFormula>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{3C6F5A4F-73EA-45E7-87BB-37AB4997CF61}" name="Quantidade Vendida"/>
+    <tableColumn id="6" xr3:uid="{1B4BCCD1-849F-41FE-B38F-0C45630FAFDF}" name="Quantidade Atual" dataDxfId="14">
+      <calculatedColumnFormula>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{B347FC4C-1C5A-4E5F-85DB-5FA2798D7D01}" name="Situação" totalsRowFunction="count" dataDxfId="13">
+      <calculatedColumnFormula>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1254,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:B13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,9 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2396,13 +2572,545 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" s="16" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="18">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>150</v>
+      </c>
+      <c r="G5">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>165</v>
+      </c>
+      <c r="H5" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="18">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>60</v>
+      </c>
+      <c r="H6" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>450</v>
+      </c>
+      <c r="G7">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>450</v>
+      </c>
+      <c r="H7" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>100</v>
+      </c>
+      <c r="H8" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="18">
+        <v>150</v>
+      </c>
+      <c r="E9">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>150</v>
+      </c>
+      <c r="H9" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="18">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>15</v>
+      </c>
+      <c r="H10" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Comprar</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="18">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>150</v>
+      </c>
+      <c r="G11">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>175</v>
+      </c>
+      <c r="H11" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="18">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>150</v>
+      </c>
+      <c r="G12">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>150</v>
+      </c>
+      <c r="H12" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="18">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>300</v>
+      </c>
+      <c r="G13">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>300</v>
+      </c>
+      <c r="H13" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="18">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>130</v>
+      </c>
+      <c r="H14" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>100</v>
+      </c>
+      <c r="H15" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="18">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>150</v>
+      </c>
+      <c r="G16">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>150</v>
+      </c>
+      <c r="H16" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="18">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>570</v>
+      </c>
+      <c r="G17">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>570</v>
+      </c>
+      <c r="H17" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>110</v>
+      </c>
+      <c r="G18">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>110</v>
+      </c>
+      <c r="H18" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="18">
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>39</v>
+      </c>
+      <c r="H19" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Atenção</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="18">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>300</v>
+      </c>
+      <c r="G20">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>300</v>
+      </c>
+      <c r="H20" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="18">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>50</v>
+      </c>
+      <c r="H21" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="18">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>10</v>
+      </c>
+      <c r="H22" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Comprar</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="18">
+        <v>100</v>
+      </c>
+      <c r="E23">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>100</v>
+      </c>
+      <c r="H23" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="18">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>200</v>
+      </c>
+      <c r="G24">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>200</v>
+      </c>
+      <c r="H24" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="18">
+        <v>30</v>
+      </c>
+      <c r="E25">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>30</v>
+      </c>
+      <c r="H25" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Atenção</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="18">
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>50</v>
+      </c>
+      <c r="H26" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="18">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>80</v>
+      </c>
+      <c r="G27">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>80</v>
+      </c>
+      <c r="H27" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="18">
+        <v>20</v>
+      </c>
+      <c r="E28">
+        <f>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</f>
+        <v>20</v>
+      </c>
+      <c r="H28" t="str">
+        <f>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</f>
+        <v>Comprar</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H5:H28">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Comprar">
+      <formula>NOT(ISERROR(SEARCH("Comprar",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Atenção">
+      <formula>NOT(ISERROR(SEARCH("Atenção",H5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2467,7 +3175,7 @@
   <dimension ref="M6:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:P6"/>
+      <selection activeCell="M7" sqref="M7:M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Data da última compra (solução para o PROCV) - Projeto
</commit_message>
<xml_diff>
--- a/Projeto/Projeto - Controle Mercado.xlsx
+++ b/Projeto/Projeto - Controle Mercado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zero\Desktop\Curso-Excel\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7108EB-18A7-467E-86F2-1AD9E26118A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12D3956-8DEC-4095-A6D6-E94DFDF40DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,6 +43,63 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>zero</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{9B668FED-24AB-4179-82AE-7257BFF83955}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>zero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Exibindo por meio do =índice que busca em determinada matriz, em determinada linha fornecida pelo retorno de corresp(onde pega o valor procurado e finda em uma matriz procurada -&gt; retornando o número da linha no find)
+finalizando o match da fórmula fornecendo qual coluna findar -&gt; matriz, núm linha, núm colunm</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="110">
   <si>
@@ -380,12 +437,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +487,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -488,7 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -525,27 +594,18 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="13">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -560,69 +620,6 @@
           <bgColor rgb="FFFF5050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1113,18 +1110,18 @@
     <sortCondition descending="1" ref="B4:B26"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{70F01BB3-039F-4F6A-9127-0FE396F11917}" name="Data" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{70F01BB3-039F-4F6A-9127-0FE396F11917}" name="Data" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{23FDBB76-891B-4BEF-88E5-CF45534E4FA6}" name="Fornecedor"/>
     <tableColumn id="3" xr3:uid="{47E77675-1CB5-4223-999C-CD7D30DA4298}" name="Mercadoria"/>
-    <tableColumn id="4" xr3:uid="{50509D53-9FDE-434A-A21C-765E6322AE8A}" name="Medida" dataDxfId="21">
+    <tableColumn id="4" xr3:uid="{50509D53-9FDE-434A-A21C-765E6322AE8A}" name="Medida" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela2[[#This Row],[Mercadoria]],cálculos!$M$7:$P$34,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{FF08DCA9-D260-4B65-9D79-32D0EDA3AD9A}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{BDD50E25-5158-4F1F-BC90-ABBF12938393}" name="Preço Unitário" dataDxfId="20" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{BDD50E25-5158-4F1F-BC90-ABBF12938393}" name="Preço Unitário" dataDxfId="10" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela2[[#This Row],[Mercadoria]],cálculos!$M$7:$P$34,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{FBF94F4E-37BE-4D76-BDDD-D3C765A36413}" name="Desconto" dataCellStyle="Porcentagem"/>
-    <tableColumn id="8" xr3:uid="{AEFD3C74-15EE-4D2B-9559-6E09557523AE}" name="Valor Pago" dataDxfId="19" dataCellStyle="Moeda">
+    <tableColumn id="8" xr3:uid="{AEFD3C74-15EE-4D2B-9559-6E09557523AE}" name="Valor Pago" dataDxfId="9" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1136,9 +1133,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4260D52-81F2-4162-98BF-30718AC2EAF3}" name="Tabela4" displayName="Tabela4" ref="B4:E9" totalsRowShown="0">
   <autoFilter ref="B4:E9" xr:uid="{C4260D52-81F2-4162-98BF-30718AC2EAF3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3DE2EC2D-FE65-43D5-9E03-63CA32193761}" name="Investimento" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{129E839C-F6BB-4D91-906F-D4AE5BA48C18}" name="Data" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{81A341C0-EC03-4544-8A0B-6ECB312FEAC6}" name="Descrição" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{3DE2EC2D-FE65-43D5-9E03-63CA32193761}" name="Investimento" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{129E839C-F6BB-4D91-906F-D4AE5BA48C18}" name="Data" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{81A341C0-EC03-4544-8A0B-6ECB312FEAC6}" name="Descrição" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{8DA02AF3-1548-4A14-9A42-6E5373D624E7}" name="Valor" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1150,16 +1147,18 @@
   <autoFilter ref="B4:H28" xr:uid="{64CF6E44-08DA-45E7-A768-DF394F8148AD}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{46C366B8-BE15-4500-9E9A-C4C93EDADFBF}" name="Produto" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{9D624FE4-2073-40B5-AD69-FB6399F49BF6}" name="Data da Última Compra"/>
+    <tableColumn id="2" xr3:uid="{9D624FE4-2073-40B5-AD69-FB6399F49BF6}" name="Data da Última Compra" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="3" xr3:uid="{34D575FB-E869-42B1-9733-C1CFD882C0FC}" name="Quantidade Inicial"/>
-    <tableColumn id="4" xr3:uid="{28E8EF48-C2E8-4765-B5A6-39213CF6B625}" name="Quantidade Comprada" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{28E8EF48-C2E8-4765-B5A6-39213CF6B625}" name="Quantidade Comprada" dataDxfId="3">
       <calculatedColumnFormula>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{3C6F5A4F-73EA-45E7-87BB-37AB4997CF61}" name="Quantidade Vendida"/>
-    <tableColumn id="6" xr3:uid="{1B4BCCD1-849F-41FE-B38F-0C45630FAFDF}" name="Quantidade Atual" dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{1B4BCCD1-849F-41FE-B38F-0C45630FAFDF}" name="Quantidade Atual" dataDxfId="2">
       <calculatedColumnFormula>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B347FC4C-1C5A-4E5F-85DB-5FA2798D7D01}" name="Situação" totalsRowFunction="count" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{B347FC4C-1C5A-4E5F-85DB-5FA2798D7D01}" name="Situação" totalsRowFunction="count" dataDxfId="1">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1799,7 +1798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2571,11 +2572,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,6 +2622,10 @@
       <c r="B5" t="s">
         <v>30</v>
       </c>
+      <c r="C5" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42187</v>
+      </c>
       <c r="D5" s="18">
         <v>15</v>
       </c>
@@ -2641,6 +2646,10 @@
       <c r="B6" t="s">
         <v>39</v>
       </c>
+      <c r="C6" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42188</v>
+      </c>
       <c r="D6" s="18">
         <v>10</v>
       </c>
@@ -2661,6 +2670,10 @@
       <c r="B7" t="s">
         <v>27</v>
       </c>
+      <c r="C7" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42189</v>
+      </c>
       <c r="D7" s="18">
         <v>0</v>
       </c>
@@ -2681,6 +2694,10 @@
       <c r="B8" t="s">
         <v>44</v>
       </c>
+      <c r="C8" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42188</v>
+      </c>
       <c r="D8" s="18">
         <v>0</v>
       </c>
@@ -2701,6 +2718,10 @@
       <c r="B9" t="s">
         <v>47</v>
       </c>
+      <c r="C9" s="14" t="str">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v/>
+      </c>
       <c r="D9" s="18">
         <v>150</v>
       </c>
@@ -2721,6 +2742,10 @@
       <c r="B10" t="s">
         <v>43</v>
       </c>
+      <c r="C10" s="14" t="str">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v/>
+      </c>
       <c r="D10" s="18">
         <v>15</v>
       </c>
@@ -2741,6 +2766,10 @@
       <c r="B11" t="s">
         <v>31</v>
       </c>
+      <c r="C11" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42187</v>
+      </c>
       <c r="D11" s="18">
         <v>25</v>
       </c>
@@ -2761,6 +2790,10 @@
       <c r="B12" t="s">
         <v>37</v>
       </c>
+      <c r="C12" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42187</v>
+      </c>
       <c r="D12" s="18">
         <v>0</v>
       </c>
@@ -2781,6 +2814,10 @@
       <c r="B13" t="s">
         <v>40</v>
       </c>
+      <c r="C13" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42189</v>
+      </c>
       <c r="D13" s="18">
         <v>0</v>
       </c>
@@ -2801,6 +2838,10 @@
       <c r="B14" t="s">
         <v>45</v>
       </c>
+      <c r="C14" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42188</v>
+      </c>
       <c r="D14" s="18">
         <v>30</v>
       </c>
@@ -2821,6 +2862,10 @@
       <c r="B15" t="s">
         <v>46</v>
       </c>
+      <c r="C15" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42188</v>
+      </c>
       <c r="D15" s="18">
         <v>0</v>
       </c>
@@ -2841,6 +2886,10 @@
       <c r="B16" t="s">
         <v>42</v>
       </c>
+      <c r="C16" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42190</v>
+      </c>
       <c r="D16" s="18">
         <v>0</v>
       </c>
@@ -2861,6 +2910,10 @@
       <c r="B17" t="s">
         <v>28</v>
       </c>
+      <c r="C17" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42190</v>
+      </c>
       <c r="D17" s="18">
         <v>0</v>
       </c>
@@ -2881,6 +2934,10 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
+      <c r="C18" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42188</v>
+      </c>
       <c r="D18" s="18">
         <v>0</v>
       </c>
@@ -2901,6 +2958,10 @@
       <c r="B19" t="s">
         <v>76</v>
       </c>
+      <c r="C19" s="14" t="str">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v/>
+      </c>
       <c r="D19" s="18">
         <v>39</v>
       </c>
@@ -2921,6 +2982,10 @@
       <c r="B20" t="s">
         <v>81</v>
       </c>
+      <c r="C20" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42188</v>
+      </c>
       <c r="D20" s="18">
         <v>0</v>
       </c>
@@ -2941,6 +3006,10 @@
       <c r="B21" t="s">
         <v>33</v>
       </c>
+      <c r="C21" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42188</v>
+      </c>
       <c r="D21" s="18">
         <v>0</v>
       </c>
@@ -2961,6 +3030,10 @@
       <c r="B22" t="s">
         <v>34</v>
       </c>
+      <c r="C22" s="14" t="str">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v/>
+      </c>
       <c r="D22" s="18">
         <v>10</v>
       </c>
@@ -2981,6 +3054,10 @@
       <c r="B23" t="s">
         <v>82</v>
       </c>
+      <c r="C23" s="14" t="str">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v/>
+      </c>
       <c r="D23" s="18">
         <v>100</v>
       </c>
@@ -3001,6 +3078,10 @@
       <c r="B24" t="s">
         <v>36</v>
       </c>
+      <c r="C24" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42189</v>
+      </c>
       <c r="D24" s="18">
         <v>0</v>
       </c>
@@ -3021,6 +3102,10 @@
       <c r="B25" t="s">
         <v>29</v>
       </c>
+      <c r="C25" s="14" t="str">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v/>
+      </c>
       <c r="D25" s="18">
         <v>30</v>
       </c>
@@ -3041,6 +3126,10 @@
       <c r="B26" t="s">
         <v>38</v>
       </c>
+      <c r="C26" s="14" t="str">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v/>
+      </c>
       <c r="D26" s="18">
         <v>50</v>
       </c>
@@ -3061,6 +3150,10 @@
       <c r="B27" t="s">
         <v>35</v>
       </c>
+      <c r="C27" s="14">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v>42187</v>
+      </c>
       <c r="D27" s="18">
         <v>0</v>
       </c>
@@ -3081,6 +3174,10 @@
       <c r="B28" t="s">
         <v>41</v>
       </c>
+      <c r="C28" s="14" t="str">
+        <f>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</f>
+        <v/>
+      </c>
       <c r="D28" s="18">
         <v>20</v>
       </c>
@@ -3099,17 +3196,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H5:H28">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Comprar">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Comprar">
       <formula>NOT(ISERROR(SEARCH("Comprar",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Atenção">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Atenção">
       <formula>NOT(ISERROR(SEARCH("Atenção",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3172,10 +3270,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="M6:P30"/>
+  <dimension ref="J6:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:M30"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3186,7 +3284,11 @@
     <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f>INDEX(M7:P30,5,2)</f>
+        <v>1.0900000000000001</v>
+      </c>
       <c r="M6" s="8" t="s">
         <v>70</v>
       </c>
@@ -3200,7 +3302,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="10:16" x14ac:dyDescent="0.25">
       <c r="M7" t="s">
         <v>30</v>
       </c>
@@ -3214,7 +3316,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f>MATCH(M17,M7:M30,0)</f>
+        <v>11</v>
+      </c>
       <c r="M8" t="s">
         <v>39</v>
       </c>
@@ -3228,7 +3334,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="10:16" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
         <v>27</v>
       </c>
@@ -3242,7 +3348,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f>MATCH(22.23,N7:N30,0)</f>
+        <v>17</v>
+      </c>
       <c r="M10" t="s">
         <v>44</v>
       </c>
@@ -3256,7 +3366,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="10:16" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
         <v>47</v>
       </c>
@@ -3270,7 +3380,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J12" t="str" cm="1">
+        <f t="array" ref="J12">INDEX(M7:P30,J10,1)</f>
+        <v>Peixe</v>
+      </c>
       <c r="M12" t="s">
         <v>43</v>
       </c>
@@ -3284,7 +3398,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="10:16" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
         <v>31</v>
       </c>
@@ -3298,7 +3412,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="10:16" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
         <v>37</v>
       </c>
@@ -3312,7 +3426,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="10:16" x14ac:dyDescent="0.25">
       <c r="M15" t="s">
         <v>40</v>
       </c>
@@ -3326,7 +3440,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="10:16" x14ac:dyDescent="0.25">
       <c r="M16" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Aba Vendas (2 de 4) - Fórmula FREQUÊNCIA - Projeto
</commit_message>
<xml_diff>
--- a/Projeto/Projeto - Controle Mercado.xlsx
+++ b/Projeto/Projeto - Controle Mercado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zero\Desktop\Curso-Excel\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB2330C-68F3-469C-8BBE-21DBB5A9BC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159DFB56-2C3C-497A-926F-4C6573396229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -83,8 +83,232 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>zero</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{BDFD29C0-3465-4A41-9728-310A15BEEBDA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>zero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fórmula soma-se-frequência ideal para contabilizar quantos id únicos temos em determinado intervalo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M33" authorId="0" shapeId="0" xr:uid="{39984DEC-C3CE-4799-ADAE-DC4F0BC7E1E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>zero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+zero:
+Fórmula soma-se-frequência ideal para contabilizar quantos id únicos temos em determinado intervalo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>zero</author>
+  </authors>
+  <commentList>
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{89D60A00-662C-4239-8BA1-931D0BD7BA6C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>zero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+zero:
+Fórmula soma-se-frequência ideal para contabilizar quantos id únicos temos em determinado intervalo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>zero</author>
+  </authors>
+  <commentList>
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{EB29B72D-47C1-4F2C-9B5F-FBB5E2E6A843}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>zero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+zero:
+Fórmula soma-se-frequência ideal para contabilizar quantos id únicos temos em determinado intervalo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q21" authorId="0" shapeId="0" xr:uid="{210251A8-8747-4476-A350-DD181D82F2D5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>zero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+zero:
+Fórmula soma-se-frequência ideal para contabilizar quantos id únicos temos em determinado intervalo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>zero</author>
+  </authors>
+  <commentList>
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{9D99FA89-B8FD-4387-B093-ABB0BB01C925}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>zero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+zero:
+Fórmula soma-se-frequência ideal para contabilizar quantos id únicos temos em determinado intervalo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>zero</author>
+  </authors>
+  <commentList>
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{08F33D39-7FB9-455E-BD24-AD5DA8EC23DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>zero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+zero:
+Fórmula soma-se-frequência ideal para contabilizar quantos id únicos temos em determinado intervalo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -106,7 +330,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="140">
   <si>
     <t>Resultados</t>
   </si>
@@ -511,6 +735,21 @@
   </si>
   <si>
     <t>Total de vendas semana 5</t>
+  </si>
+  <si>
+    <t>Ticket Médio</t>
+  </si>
+  <si>
+    <t>Vendas por Entrega (%)</t>
+  </si>
+  <si>
+    <t>Vendas por Entrega (R$)</t>
+  </si>
+  <si>
+    <t>Receita de Entregas (R$)</t>
+  </si>
+  <si>
+    <t>Número de Vendas</t>
   </si>
 </sst>
 </file>
@@ -521,7 +760,7 @@
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,15 +834,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="9"/>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="9"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -611,10 +848,22 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -812,7 +1061,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -857,18 +1106,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -877,20 +1127,6 @@
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="45">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -1025,6 +1261,20 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3442,18 +3692,18 @@
   <autoFilter ref="B4:H28" xr:uid="{64CF6E44-08DA-45E7-A768-DF394F8148AD}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{46C366B8-BE15-4500-9E9A-C4C93EDADFBF}" name="Produto" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{9D624FE4-2073-40B5-AD69-FB6399F49BF6}" name="Data da Última Compra" dataDxfId="37">
+    <tableColumn id="2" xr3:uid="{9D624FE4-2073-40B5-AD69-FB6399F49BF6}" name="Data da Última Compra" dataDxfId="35">
       <calculatedColumnFormula>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{34D575FB-E869-42B1-9733-C1CFD882C0FC}" name="Quantidade Inicial"/>
-    <tableColumn id="4" xr3:uid="{28E8EF48-C2E8-4765-B5A6-39213CF6B625}" name="Quantidade Comprada" dataDxfId="36">
+    <tableColumn id="4" xr3:uid="{28E8EF48-C2E8-4765-B5A6-39213CF6B625}" name="Quantidade Comprada" dataDxfId="34">
       <calculatedColumnFormula>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{3C6F5A4F-73EA-45E7-87BB-37AB4997CF61}" name="Quantidade Vendida"/>
-    <tableColumn id="6" xr3:uid="{1B4BCCD1-849F-41FE-B38F-0C45630FAFDF}" name="Quantidade Atual" dataDxfId="35">
+    <tableColumn id="6" xr3:uid="{1B4BCCD1-849F-41FE-B38F-0C45630FAFDF}" name="Quantidade Atual" dataDxfId="33">
       <calculatedColumnFormula>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B347FC4C-1C5A-4E5F-85DB-5FA2798D7D01}" name="Situação" totalsRowFunction="count" dataDxfId="34">
+    <tableColumn id="7" xr3:uid="{B347FC4C-1C5A-4E5F-85DB-5FA2798D7D01}" name="Situação" totalsRowFunction="count" dataDxfId="32">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3469,27 +3719,27 @@
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{3737DABE-D6EE-4F59-A12C-034FE441E40A}" name="Id da Venda"/>
-    <tableColumn id="2" xr3:uid="{37F6714B-5309-4E75-AC83-CA137426F275}" name="Data" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{37F6714B-5309-4E75-AC83-CA137426F275}" name="Data" dataDxfId="31"/>
     <tableColumn id="3" xr3:uid="{098A8685-426F-4B00-8B9A-AC231D18B90F}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{260E818A-3D97-43C5-AA6F-6AD331804B75}" name="Medida" dataDxfId="32">
+    <tableColumn id="4" xr3:uid="{260E818A-3D97-43C5-AA6F-6AD331804B75}" name="Medida" dataDxfId="30">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{059DA008-4A32-4057-812C-3D932A132A79}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{8166E928-B434-47CA-99B0-709F3F85DA94}" name="Preço Unitário" dataDxfId="31" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{8166E928-B434-47CA-99B0-709F3F85DA94}" name="Preço Unitário" dataDxfId="29" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5B0D52A9-73ED-4B29-AC74-D34DD4ECBFBA}" name="SubTotal" dataDxfId="30" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{5B0D52A9-73ED-4B29-AC74-D34DD4ECBFBA}" name="SubTotal" dataDxfId="28" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela5[[#This Row],[Preço Unitário]]*Tabela5[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0FA4A39A-7392-4DAF-B8AD-9CDA986D4740}" name="Desconto" dataDxfId="29" dataCellStyle="Porcentagem"/>
+    <tableColumn id="8" xr3:uid="{0FA4A39A-7392-4DAF-B8AD-9CDA986D4740}" name="Desconto" dataDxfId="27" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{F725BE9C-C71B-49D8-B12C-03F7062FB43E}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{A1F728EA-36F0-45F2-8E8C-0DE5B31DAE1D}" name="Valor de Entrega" dataDxfId="28" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{A1F728EA-36F0-45F2-8E8C-0DE5B31DAE1D}" name="Valor de Entrega" dataDxfId="26" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela5[[#This Row],[Id da Venda]]=B6,0,VLOOKUP(Tabela5[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FB59B27A-F13E-4079-866F-8BBBE1ADE501}" name="Total" dataDxfId="27" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{FB59B27A-F13E-4079-866F-8BBBE1ADE501}" name="Total" dataDxfId="25" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela5[[#This Row],[SubTotal]]*(1 - Tabela5[[#This Row],[Desconto]])+Tabela5[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F41EE8F0-5091-4212-AB61-6A6BB81E06EA}" name="Total para o Cliente" dataDxfId="26" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{F41EE8F0-5091-4212-AB61-6A6BB81E06EA}" name="Total para o Cliente" dataDxfId="24" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela5[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela5[Id da Venda],Tabela5[[#This Row],[Id da Venda]],Tabela5[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3504,25 +3754,25 @@
     <tableColumn id="1" xr3:uid="{EF7D5F4F-E81D-4B69-8CDD-E570A7D9D93A}" name="Id da Venda"/>
     <tableColumn id="2" xr3:uid="{2B6FC9F5-E966-4CFF-98AF-CBBE8CEB93FE}" name="Data"/>
     <tableColumn id="3" xr3:uid="{856465FB-BF97-4416-8BB3-C3ACF7D41AA6}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{DD38D336-5E77-46E1-9B33-BF93FC0E788C}" name="Medida" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{DD38D336-5E77-46E1-9B33-BF93FC0E788C}" name="Medida" dataDxfId="23">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela57[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{AD93DD2E-782E-4666-B095-0BE2EDC800D0}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{49B276E8-AF1C-4EB9-A19B-4E32AA04FEFD}" name="Preço Unitário" dataDxfId="24" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{49B276E8-AF1C-4EB9-A19B-4E32AA04FEFD}" name="Preço Unitário" dataDxfId="22" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela57[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{609C5A11-606B-46DF-87F4-D62A4539BDEC}" name="SubTotal" dataDxfId="23" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{609C5A11-606B-46DF-87F4-D62A4539BDEC}" name="SubTotal" dataDxfId="21" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela57[[#This Row],[Preço Unitário]]*Tabela57[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{02E3827B-C0A7-4EB6-9714-8C45E1805E50}" name="Desconto" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{18E066A9-A495-4229-91F2-958EE9A77257}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{868D6B54-6FCE-444C-9A98-327F8252289B}" name="Valor de Entrega" dataDxfId="22" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{868D6B54-6FCE-444C-9A98-327F8252289B}" name="Valor de Entrega" dataDxfId="20" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela57[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7CF1F82D-735D-402F-B0CF-B3FE1FCD42BE}" name="Total" dataDxfId="21" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{7CF1F82D-735D-402F-B0CF-B3FE1FCD42BE}" name="Total" dataDxfId="19" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela57[[#This Row],[SubTotal]]*(1 - Tabela57[[#This Row],[Desconto]])+Tabela57[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A839CEB0-FFD4-473A-B9DD-173894133EF3}" name="Total para o Cliente" dataDxfId="20" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{A839CEB0-FFD4-473A-B9DD-173894133EF3}" name="Total para o Cliente" dataDxfId="18" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela57[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela57[Id da Venda],Tabela57[[#This Row],[Id da Venda]],Tabela57[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3537,25 +3787,25 @@
     <tableColumn id="1" xr3:uid="{9DFB229B-DA21-4029-A82D-6469CB1FD9C3}" name="Id da Venda"/>
     <tableColumn id="2" xr3:uid="{D1D96CF1-90F1-4E06-B6D2-77A8F5050BF4}" name="Data"/>
     <tableColumn id="3" xr3:uid="{63903A64-01C2-4183-81ED-62F5971C61B2}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{5AEE8A70-0BE2-4C9B-909B-D6311A223E94}" name="Medida" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{5AEE8A70-0BE2-4C9B-909B-D6311A223E94}" name="Medida" dataDxfId="17">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela58[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{D9D3FB24-2C9C-409B-ACEE-7FFC875B7663}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{D0F473B5-1921-47BF-B8F9-EBC560004371}" name="Preço Unitário" dataDxfId="18" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{D0F473B5-1921-47BF-B8F9-EBC560004371}" name="Preço Unitário" dataDxfId="16" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela58[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8A7B683E-1EE9-49AD-9A38-2F14490713B3}" name="SubTotal" dataDxfId="17" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{8A7B683E-1EE9-49AD-9A38-2F14490713B3}" name="SubTotal" dataDxfId="15" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela58[[#This Row],[Preço Unitário]]*Tabela58[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{2609A5E7-65E1-40F1-A55D-4A085B5458D5}" name="Desconto" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{B60D6E5B-8DAB-4FEE-B47A-6746ED368BFC}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{1AA1BBEB-FA48-4868-B788-3BE480EC3641}" name="Valor de Entrega" dataDxfId="16" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{1AA1BBEB-FA48-4868-B788-3BE480EC3641}" name="Valor de Entrega" dataDxfId="14" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela58[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D1A75EBE-1E56-4116-9973-B379F1A5E6F0}" name="Total" dataDxfId="15" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{D1A75EBE-1E56-4116-9973-B379F1A5E6F0}" name="Total" dataDxfId="13" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela58[[#This Row],[SubTotal]]*(1 - Tabela58[[#This Row],[Desconto]])+Tabela58[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{DAEC0DE5-B891-47A0-8B19-5307A968E3CC}" name="Total para o Cliente" dataDxfId="14" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{DAEC0DE5-B891-47A0-8B19-5307A968E3CC}" name="Total para o Cliente" dataDxfId="12" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela58[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela58[Id da Venda],Tabela58[[#This Row],[Id da Venda]],Tabela58[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3570,25 +3820,25 @@
     <tableColumn id="1" xr3:uid="{BAD241FC-FEF6-4531-BB4B-2B112245EC84}" name="Id da Venda"/>
     <tableColumn id="2" xr3:uid="{4213A27C-100E-4E40-B852-6DAD63221A71}" name="Data"/>
     <tableColumn id="3" xr3:uid="{FBB10A83-F749-4D61-BA4D-9A6533B7FEB8}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{E8FA974C-0C3B-401A-B6FD-25063F2E6478}" name="Medida" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{E8FA974C-0C3B-401A-B6FD-25063F2E6478}" name="Medida" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela59[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{93E6AF85-0AA0-4B14-9513-91ED7FB3602A}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{A01183EB-74C9-4E6B-B3A8-532DAE9C0EC9}" name="Preço Unitário" dataDxfId="12" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{A01183EB-74C9-4E6B-B3A8-532DAE9C0EC9}" name="Preço Unitário" dataDxfId="10" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela59[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{24DCBB98-DF97-4E91-88B7-EB3FF4AACAA6}" name="SubTotal" dataDxfId="11" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{24DCBB98-DF97-4E91-88B7-EB3FF4AACAA6}" name="SubTotal" dataDxfId="9" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela59[[#This Row],[Preço Unitário]]*Tabela59[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{71CEAB54-BC14-4977-9F4A-9AE74EFCF934}" name="Desconto" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{AEE7F2D7-AF98-4C33-80C6-8AE18239157E}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{E043D4D8-B241-41EB-9FA2-28B03F0464A1}" name="Valor de Entrega" dataDxfId="10" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{E043D4D8-B241-41EB-9FA2-28B03F0464A1}" name="Valor de Entrega" dataDxfId="8" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela59[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D00BD8CD-4E8D-4099-A6AF-DC6C39383E89}" name="Total" dataDxfId="9" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{D00BD8CD-4E8D-4099-A6AF-DC6C39383E89}" name="Total" dataDxfId="7" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela59[[#This Row],[SubTotal]]*(1 - Tabela59[[#This Row],[Desconto]])+Tabela59[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{FA37B1A0-582E-493C-BDB3-028730689B4F}" name="Total para o Cliente" dataDxfId="8" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{FA37B1A0-582E-493C-BDB3-028730689B4F}" name="Total para o Cliente" dataDxfId="6" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela59[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela59[Id da Venda],Tabela59[[#This Row],[Id da Venda]],Tabela59[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3603,25 +3853,25 @@
     <tableColumn id="1" xr3:uid="{0FCFF496-1814-410F-ABF4-CB2A27F6C181}" name="Id da Venda"/>
     <tableColumn id="2" xr3:uid="{D98BEDD6-0C49-4F7A-8A6B-F1A8275F59BB}" name="Data"/>
     <tableColumn id="3" xr3:uid="{2497BEF2-F9CC-479D-944E-75AFB9C63334}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{95F6C9B9-35CA-45A8-BCB1-58B84AB19A5A}" name="Medida" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{95F6C9B9-35CA-45A8-BCB1-58B84AB19A5A}" name="Medida" dataDxfId="5">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5910[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{6BEBE7C6-A3F7-4015-B659-714498201054}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{A0018570-D78F-4AF7-863D-4A87B33FFEB6}" name="Preço Unitário" dataDxfId="6" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{A0018570-D78F-4AF7-863D-4A87B33FFEB6}" name="Preço Unitário" dataDxfId="4" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5910[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{21D8DD35-CDAC-4A87-A570-E4AC6842F334}" name="SubTotal" dataDxfId="5" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{21D8DD35-CDAC-4A87-A570-E4AC6842F334}" name="SubTotal" dataDxfId="3" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela5910[[#This Row],[Preço Unitário]]*Tabela5910[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{45C60647-4AFD-46F9-BBCB-D010B8C4D5A3}" name="Desconto" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{67B3CCC2-89B9-4DE5-8561-05A98ABA1597}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{E679215B-C7A3-48DE-B602-5AE0FBCAAAE5}" name="Valor de Entrega" dataDxfId="4" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{E679215B-C7A3-48DE-B602-5AE0FBCAAAE5}" name="Valor de Entrega" dataDxfId="2" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5910[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{043824D5-311C-4DEE-A15B-7E0406417187}" name="Total" dataDxfId="3" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{043824D5-311C-4DEE-A15B-7E0406417187}" name="Total" dataDxfId="1" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela5910[[#This Row],[SubTotal]]*(1 - Tabela5910[[#This Row],[Desconto]])+Tabela5910[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{9F29B0E6-5B32-42BC-ABD3-C98CAF68E066}" name="Total para o Cliente" dataDxfId="2" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{9F29B0E6-5B32-42BC-ABD3-C98CAF68E066}" name="Total para o Cliente" dataDxfId="0" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela5910[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela5910[Id da Venda],Tabela5910[[#This Row],[Id da Venda]],Tabela5910[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3935,11 +4185,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4458DA11-EF8A-4DC2-9022-6C68CB4E3E5F}">
-  <dimension ref="B2:M18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4458DA11-EF8A-4DC2-9022-6C68CB4E3E5F}">
+  <dimension ref="B2:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B19" sqref="B19:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4288,7 +4538,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B17" s="20" t="s">
         <v>123</v>
       </c>
@@ -4307,7 +4557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B18" s="22" t="s">
         <v>124</v>
       </c>
@@ -4326,11 +4576,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B19" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="46" cm="1">
+        <f t="array" ref="M19">SUM(IF(FREQUENCY(Tabela58[Id da Venda],Tabela58[Id da Venda])&gt;0,1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="F21" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="46" cm="1">
+        <f t="array" ref="Q21">SUM(IF(FREQUENCY(Tabela57[Id da Venda],Tabela57[Id da Venda])&gt;0,1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4354,11 +4643,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD89CF8-2CAA-4F58-8B64-AB3B1354D793}">
-  <dimension ref="B2:M18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD89CF8-2CAA-4F58-8B64-AB3B1354D793}">
+  <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4745,11 +5034,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B19" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="46" cm="1">
+        <f t="array" ref="M19">SUM(IF(FREQUENCY(Tabela59[Id da Venda],Tabela59[Id da Venda])&gt;0,1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4773,11 +5082,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C877A8-E5B9-4F21-9019-7D4DD012F5E6}">
-  <dimension ref="B2:M18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C877A8-E5B9-4F21-9019-7D4DD012F5E6}">
+  <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5164,11 +5473,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B19" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="46" cm="1">
+        <f t="array" ref="M19">SUM(IF(FREQUENCY(Tabela5910[Id da Venda],Tabela5910[Id da Venda])&gt;0,1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -5195,8 +5524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B6:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5402,6 +5731,13 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16" cm="1">
+        <f t="array" ref="D16">SUM(IF(FREQUENCY(B16:B23,B16:B23)&gt;0,1,0))</f>
+        <v>6</v>
+      </c>
       <c r="M16" t="s">
         <v>44</v>
       </c>
@@ -5415,7 +5751,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>7</v>
+      </c>
       <c r="M17" t="s">
         <v>45</v>
       </c>
@@ -5429,7 +5768,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
       <c r="M18" t="s">
         <v>41</v>
       </c>
@@ -5443,7 +5785,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
       <c r="M19" t="s">
         <v>27</v>
       </c>
@@ -5457,7 +5802,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2</v>
+      </c>
       <c r="M20" t="s">
         <v>31</v>
       </c>
@@ -5471,7 +5819,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>3</v>
+      </c>
       <c r="M21" t="s">
         <v>75</v>
       </c>
@@ -5485,7 +5836,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>5</v>
+      </c>
       <c r="M22" t="s">
         <v>80</v>
       </c>
@@ -5499,7 +5853,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>4</v>
+      </c>
       <c r="M23" t="s">
         <v>32</v>
       </c>
@@ -5513,7 +5870,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
         <v>33</v>
       </c>
@@ -5527,7 +5884,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
         <v>81</v>
       </c>
@@ -5541,7 +5898,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M26" t="s">
         <v>35</v>
       </c>
@@ -5555,7 +5912,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
         <v>28</v>
       </c>
@@ -5569,7 +5926,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
         <v>37</v>
       </c>
@@ -5583,7 +5940,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M29" t="s">
         <v>34</v>
       </c>
@@ -5597,7 +5954,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M30" t="s">
         <v>40</v>
       </c>
@@ -7347,10 +7704,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H5:H28">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Atenção">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="Atenção">
       <formula>NOT(ISERROR(SEARCH("Atenção",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Comprar">
+    <cfRule type="containsText" dxfId="36" priority="3" operator="containsText" text="Comprar">
       <formula>NOT(ISERROR(SEARCH("Comprar",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7399,10 +7756,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B1:O22"/>
+  <dimension ref="B1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7421,7 +7778,7 @@
     </row>
     <row r="3" spans="2:15" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="O5" s="45" t="s">
+      <c r="O5" s="36" t="s">
         <v>129</v>
       </c>
     </row>
@@ -7578,10 +7935,10 @@
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="31"/>
       <c r="C15" s="27"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
@@ -7594,10 +7951,10 @@
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="31"/>
       <c r="C16" s="27"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
@@ -7610,13 +7967,13 @@
     <row r="17" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
       <c r="C17" s="27"/>
-      <c r="D17" s="43" t="str">
+      <c r="D17" s="44" t="str">
         <f>"Total de vendas de "&amp;O5</f>
         <v>Total de vendas de Agosto</v>
       </c>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44">
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45">
         <f>SUM(G10:G14)</f>
         <v>759.7320000000002</v>
       </c>
@@ -7694,6 +8051,243 @@
       <c r="O21" s="35"/>
     </row>
     <row r="22" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="30"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="31"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="32"/>
+    </row>
+    <row r="26" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="31"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="32"/>
+    </row>
+    <row r="27" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B27" s="31"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="32"/>
+    </row>
+    <row r="28" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="31"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="40">
+        <f>SUM('Semana 1'!M32,'Semana 2'!M18,'Semana 3'!M18,'Semana 4'!M18,'Semana 5'!M18)</f>
+        <v>45.5</v>
+      </c>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="32"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="31"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="32"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="31"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="32"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="31"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="32"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="31"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="32"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="31"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="32"/>
+    </row>
+    <row r="34" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B34" s="31"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="32"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="31"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="32"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="31"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="32"/>
+    </row>
+    <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="33"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
+      <c r="O37" s="35"/>
+    </row>
+    <row r="38" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7703,11 +8297,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C552C30-8CEE-4E95-8103-1820B67CA8FF}">
-  <dimension ref="B1:M32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C552C30-8CEE-4E95-8103-1820B67CA8FF}">
+  <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8867,21 +9461,41 @@
         <v>40.5</v>
       </c>
     </row>
+    <row r="33" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B33" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="46" cm="1">
+        <f t="array" ref="M33">SUM(IF(FREQUENCY(B5:B29,B5:B29)&gt;0,1,0))</f>
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9877ADF6-D66F-4C0E-9CFA-D21ABC6AA094}">
-  <dimension ref="B2:M18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9877ADF6-D66F-4C0E-9CFA-D21ABC6AA094}">
+  <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="B19" sqref="B19:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9268,11 +9882,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="19" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B19" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="46" cm="1">
+        <f t="array" ref="M19">SUM(IF(FREQUENCY(Tabela57[Id da Venda],Tabela57[Id da Venda])&gt;0,1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
Aba Vendas (3 de 4) - Receitas e Ticket Médio - Projeto
</commit_message>
<xml_diff>
--- a/Projeto/Projeto - Controle Mercado.xlsx
+++ b/Projeto/Projeto - Controle Mercado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zero\Desktop\Curso-Excel\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159DFB56-2C3C-497A-926F-4C6573396229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582CFDC9-11F1-4142-9944-866C9D18588C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1061,7 +1061,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1119,6 +1119,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1127,6 +1129,20 @@
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -1263,20 +1279,6 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1352,39 +1354,11 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1407,8 +1381,8 @@
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1432,13 +1406,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1448,7 +1423,116 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
+              <c:f>Vendas!$C$10:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Total de vendas semana 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total de vendas semana 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total de vendas semana 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total de vendas semana 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Total de vendas semana 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>Vendas!$D$10:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD27-466B-93D5-B05232F480DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Vendas!$C$10:$C$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1480,47 +1564,19 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BD27-466B-93D5-B05232F480DA}"/>
+              <c16:uniqueId val="{00000001-BD27-466B-93D5-B05232F480DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1543,8 +1599,8 @@
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1568,13 +1624,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1584,7 +1641,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Vendas!$D$10:$D$14</c:f>
+              <c:f>Vendas!$C$10:$C$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1608,142 +1665,6 @@
           <c:val>
             <c:numRef>
               <c:f>Vendas!$F$10:$F$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BD27-466B-93D5-B05232F480DA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Vendas!$D$10:$D$14</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Total de vendas semana 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total de vendas semana 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total de vendas semana 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total de vendas semana 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Total de vendas semana 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Vendas!$G$10:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1780,8 +1701,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
         <c:axId val="1951978415"/>
         <c:axId val="1948964863"/>
       </c:barChart>
@@ -1817,8 +1738,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1876,8 +1797,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1916,7 +1837,391 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Vendas!$C$27:$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Vendas por Entrega (R$)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Receita de Entregas (R$)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Vendas!$F$27:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>435.53200000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2CE4-478E-A46D-CC810218A7C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1002969151"/>
+        <c:axId val="1002967487"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Vendas!$C$27:$C$28</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Vendas por Entrega (R$)</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Receita de Entregas (R$)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Vendas!$D$27:$D$28</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-2CE4-478E-A46D-CC810218A7C4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Vendas!$C$27:$C$28</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Vendas por Entrega (R$)</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Receita de Entregas (R$)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Vendas!$E$27:$E$28</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-2CE4-478E-A46D-CC810218A7C4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1002969151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1002967487"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1002967487"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1002969151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1940,10 +2245,47 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1977,18 +2319,18 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="206">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1996,8 +2338,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -2018,7 +2360,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2034,7 +2376,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2042,8 +2384,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2077,62 +2419,36 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="15875" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2144,33 +2460,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2187,18 +2500,20 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2213,15 +2528,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2232,17 +2547,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2251,16 +2566,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2269,15 +2585,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2296,16 +2618,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2314,17 +2637,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2333,16 +2656,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2352,8 +2676,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2363,7 +2687,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -2371,7 +2695,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2380,21 +2704,10 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2402,17 +2715,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2422,26 +2735,27 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2451,8 +2765,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2471,8 +2785,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2484,8 +2798,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2495,8 +2809,519 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3395,14 +4220,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
+      <xdr:colOff>742950</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
@@ -3424,6 +4249,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D927DE6-C913-4396-800C-254D05373E1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3692,18 +4553,18 @@
   <autoFilter ref="B4:H28" xr:uid="{64CF6E44-08DA-45E7-A768-DF394F8148AD}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{46C366B8-BE15-4500-9E9A-C4C93EDADFBF}" name="Produto" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{9D624FE4-2073-40B5-AD69-FB6399F49BF6}" name="Data da Última Compra" dataDxfId="35">
+    <tableColumn id="2" xr3:uid="{9D624FE4-2073-40B5-AD69-FB6399F49BF6}" name="Data da Última Compra" dataDxfId="37">
       <calculatedColumnFormula>IFERROR(INDEX(Tabela2[],MATCH(Tabela1[[#This Row],[Produto]],Tabela2[Mercadoria],0),1),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{34D575FB-E869-42B1-9733-C1CFD882C0FC}" name="Quantidade Inicial"/>
-    <tableColumn id="4" xr3:uid="{28E8EF48-C2E8-4765-B5A6-39213CF6B625}" name="Quantidade Comprada" dataDxfId="34">
+    <tableColumn id="4" xr3:uid="{28E8EF48-C2E8-4765-B5A6-39213CF6B625}" name="Quantidade Comprada" dataDxfId="36">
       <calculatedColumnFormula>SUMIF(Tabela2[Mercadoria],Tabela1[[#This Row],[Produto]],Tabela2[Quantidade])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{3C6F5A4F-73EA-45E7-87BB-37AB4997CF61}" name="Quantidade Vendida"/>
-    <tableColumn id="6" xr3:uid="{1B4BCCD1-849F-41FE-B38F-0C45630FAFDF}" name="Quantidade Atual" dataDxfId="33">
+    <tableColumn id="6" xr3:uid="{1B4BCCD1-849F-41FE-B38F-0C45630FAFDF}" name="Quantidade Atual" dataDxfId="35">
       <calculatedColumnFormula>Tabela1[[#This Row],[Quantidade Inicial]]+Tabela1[[#This Row],[Quantidade Comprada]]-Tabela1[[#This Row],[Quantidade Vendida]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B347FC4C-1C5A-4E5F-85DB-5FA2798D7D01}" name="Situação" totalsRowFunction="count" dataDxfId="32">
+    <tableColumn id="7" xr3:uid="{B347FC4C-1C5A-4E5F-85DB-5FA2798D7D01}" name="Situação" totalsRowFunction="count" dataDxfId="34">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;50,IF(Tabela1[[#This Row],[Quantidade Atual]]&lt;21,"Comprar","Atenção"),"Ok")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3719,27 +4580,27 @@
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{3737DABE-D6EE-4F59-A12C-034FE441E40A}" name="Id da Venda"/>
-    <tableColumn id="2" xr3:uid="{37F6714B-5309-4E75-AC83-CA137426F275}" name="Data" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{37F6714B-5309-4E75-AC83-CA137426F275}" name="Data" dataDxfId="33"/>
     <tableColumn id="3" xr3:uid="{098A8685-426F-4B00-8B9A-AC231D18B90F}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{260E818A-3D97-43C5-AA6F-6AD331804B75}" name="Medida" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{260E818A-3D97-43C5-AA6F-6AD331804B75}" name="Medida" dataDxfId="32">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{059DA008-4A32-4057-812C-3D932A132A79}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{8166E928-B434-47CA-99B0-709F3F85DA94}" name="Preço Unitário" dataDxfId="29" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{8166E928-B434-47CA-99B0-709F3F85DA94}" name="Preço Unitário" dataDxfId="31" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5B0D52A9-73ED-4B29-AC74-D34DD4ECBFBA}" name="SubTotal" dataDxfId="28" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{5B0D52A9-73ED-4B29-AC74-D34DD4ECBFBA}" name="SubTotal" dataDxfId="30" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela5[[#This Row],[Preço Unitário]]*Tabela5[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0FA4A39A-7392-4DAF-B8AD-9CDA986D4740}" name="Desconto" dataDxfId="27" dataCellStyle="Porcentagem"/>
+    <tableColumn id="8" xr3:uid="{0FA4A39A-7392-4DAF-B8AD-9CDA986D4740}" name="Desconto" dataDxfId="29" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{F725BE9C-C71B-49D8-B12C-03F7062FB43E}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{A1F728EA-36F0-45F2-8E8C-0DE5B31DAE1D}" name="Valor de Entrega" dataDxfId="26" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{A1F728EA-36F0-45F2-8E8C-0DE5B31DAE1D}" name="Valor de Entrega" dataDxfId="28" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela5[[#This Row],[Id da Venda]]=B6,0,VLOOKUP(Tabela5[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FB59B27A-F13E-4079-866F-8BBBE1ADE501}" name="Total" dataDxfId="25" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{FB59B27A-F13E-4079-866F-8BBBE1ADE501}" name="Total" dataDxfId="27" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela5[[#This Row],[SubTotal]]*(1 - Tabela5[[#This Row],[Desconto]])+Tabela5[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F41EE8F0-5091-4212-AB61-6A6BB81E06EA}" name="Total para o Cliente" dataDxfId="24" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{F41EE8F0-5091-4212-AB61-6A6BB81E06EA}" name="Total para o Cliente" dataDxfId="26" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela5[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela5[Id da Venda],Tabela5[[#This Row],[Id da Venda]],Tabela5[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3754,25 +4615,25 @@
     <tableColumn id="1" xr3:uid="{EF7D5F4F-E81D-4B69-8CDD-E570A7D9D93A}" name="Id da Venda"/>
     <tableColumn id="2" xr3:uid="{2B6FC9F5-E966-4CFF-98AF-CBBE8CEB93FE}" name="Data"/>
     <tableColumn id="3" xr3:uid="{856465FB-BF97-4416-8BB3-C3ACF7D41AA6}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{DD38D336-5E77-46E1-9B33-BF93FC0E788C}" name="Medida" dataDxfId="23">
+    <tableColumn id="4" xr3:uid="{DD38D336-5E77-46E1-9B33-BF93FC0E788C}" name="Medida" dataDxfId="25">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela57[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{AD93DD2E-782E-4666-B095-0BE2EDC800D0}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{49B276E8-AF1C-4EB9-A19B-4E32AA04FEFD}" name="Preço Unitário" dataDxfId="22" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{49B276E8-AF1C-4EB9-A19B-4E32AA04FEFD}" name="Preço Unitário" dataDxfId="24" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela57[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{609C5A11-606B-46DF-87F4-D62A4539BDEC}" name="SubTotal" dataDxfId="21" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{609C5A11-606B-46DF-87F4-D62A4539BDEC}" name="SubTotal" dataDxfId="23" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela57[[#This Row],[Preço Unitário]]*Tabela57[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{02E3827B-C0A7-4EB6-9714-8C45E1805E50}" name="Desconto" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{18E066A9-A495-4229-91F2-958EE9A77257}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{868D6B54-6FCE-444C-9A98-327F8252289B}" name="Valor de Entrega" dataDxfId="20" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{868D6B54-6FCE-444C-9A98-327F8252289B}" name="Valor de Entrega" dataDxfId="22" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela57[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7CF1F82D-735D-402F-B0CF-B3FE1FCD42BE}" name="Total" dataDxfId="19" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{7CF1F82D-735D-402F-B0CF-B3FE1FCD42BE}" name="Total" dataDxfId="21" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela57[[#This Row],[SubTotal]]*(1 - Tabela57[[#This Row],[Desconto]])+Tabela57[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A839CEB0-FFD4-473A-B9DD-173894133EF3}" name="Total para o Cliente" dataDxfId="18" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{A839CEB0-FFD4-473A-B9DD-173894133EF3}" name="Total para o Cliente" dataDxfId="20" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela57[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela57[Id da Venda],Tabela57[[#This Row],[Id da Venda]],Tabela57[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3787,25 +4648,25 @@
     <tableColumn id="1" xr3:uid="{9DFB229B-DA21-4029-A82D-6469CB1FD9C3}" name="Id da Venda"/>
     <tableColumn id="2" xr3:uid="{D1D96CF1-90F1-4E06-B6D2-77A8F5050BF4}" name="Data"/>
     <tableColumn id="3" xr3:uid="{63903A64-01C2-4183-81ED-62F5971C61B2}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{5AEE8A70-0BE2-4C9B-909B-D6311A223E94}" name="Medida" dataDxfId="17">
+    <tableColumn id="4" xr3:uid="{5AEE8A70-0BE2-4C9B-909B-D6311A223E94}" name="Medida" dataDxfId="19">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela58[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{D9D3FB24-2C9C-409B-ACEE-7FFC875B7663}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{D0F473B5-1921-47BF-B8F9-EBC560004371}" name="Preço Unitário" dataDxfId="16" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{D0F473B5-1921-47BF-B8F9-EBC560004371}" name="Preço Unitário" dataDxfId="18" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela58[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8A7B683E-1EE9-49AD-9A38-2F14490713B3}" name="SubTotal" dataDxfId="15" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{8A7B683E-1EE9-49AD-9A38-2F14490713B3}" name="SubTotal" dataDxfId="17" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela58[[#This Row],[Preço Unitário]]*Tabela58[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{2609A5E7-65E1-40F1-A55D-4A085B5458D5}" name="Desconto" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{B60D6E5B-8DAB-4FEE-B47A-6746ED368BFC}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{1AA1BBEB-FA48-4868-B788-3BE480EC3641}" name="Valor de Entrega" dataDxfId="14" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{1AA1BBEB-FA48-4868-B788-3BE480EC3641}" name="Valor de Entrega" dataDxfId="16" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela58[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D1A75EBE-1E56-4116-9973-B379F1A5E6F0}" name="Total" dataDxfId="13" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{D1A75EBE-1E56-4116-9973-B379F1A5E6F0}" name="Total" dataDxfId="15" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela58[[#This Row],[SubTotal]]*(1 - Tabela58[[#This Row],[Desconto]])+Tabela58[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{DAEC0DE5-B891-47A0-8B19-5307A968E3CC}" name="Total para o Cliente" dataDxfId="12" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{DAEC0DE5-B891-47A0-8B19-5307A968E3CC}" name="Total para o Cliente" dataDxfId="14" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela58[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela58[Id da Venda],Tabela58[[#This Row],[Id da Venda]],Tabela58[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3820,25 +4681,25 @@
     <tableColumn id="1" xr3:uid="{BAD241FC-FEF6-4531-BB4B-2B112245EC84}" name="Id da Venda"/>
     <tableColumn id="2" xr3:uid="{4213A27C-100E-4E40-B852-6DAD63221A71}" name="Data"/>
     <tableColumn id="3" xr3:uid="{FBB10A83-F749-4D61-BA4D-9A6533B7FEB8}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{E8FA974C-0C3B-401A-B6FD-25063F2E6478}" name="Medida" dataDxfId="11">
+    <tableColumn id="4" xr3:uid="{E8FA974C-0C3B-401A-B6FD-25063F2E6478}" name="Medida" dataDxfId="13">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela59[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{93E6AF85-0AA0-4B14-9513-91ED7FB3602A}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{A01183EB-74C9-4E6B-B3A8-532DAE9C0EC9}" name="Preço Unitário" dataDxfId="10" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{A01183EB-74C9-4E6B-B3A8-532DAE9C0EC9}" name="Preço Unitário" dataDxfId="12" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela59[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{24DCBB98-DF97-4E91-88B7-EB3FF4AACAA6}" name="SubTotal" dataDxfId="9" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{24DCBB98-DF97-4E91-88B7-EB3FF4AACAA6}" name="SubTotal" dataDxfId="11" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela59[[#This Row],[Preço Unitário]]*Tabela59[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{71CEAB54-BC14-4977-9F4A-9AE74EFCF934}" name="Desconto" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{AEE7F2D7-AF98-4C33-80C6-8AE18239157E}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{E043D4D8-B241-41EB-9FA2-28B03F0464A1}" name="Valor de Entrega" dataDxfId="8" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{E043D4D8-B241-41EB-9FA2-28B03F0464A1}" name="Valor de Entrega" dataDxfId="10" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela59[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D00BD8CD-4E8D-4099-A6AF-DC6C39383E89}" name="Total" dataDxfId="7" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{D00BD8CD-4E8D-4099-A6AF-DC6C39383E89}" name="Total" dataDxfId="9" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela59[[#This Row],[SubTotal]]*(1 - Tabela59[[#This Row],[Desconto]])+Tabela59[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{FA37B1A0-582E-493C-BDB3-028730689B4F}" name="Total para o Cliente" dataDxfId="6" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{FA37B1A0-582E-493C-BDB3-028730689B4F}" name="Total para o Cliente" dataDxfId="8" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela59[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela59[Id da Venda],Tabela59[[#This Row],[Id da Venda]],Tabela59[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3853,25 +4714,25 @@
     <tableColumn id="1" xr3:uid="{0FCFF496-1814-410F-ABF4-CB2A27F6C181}" name="Id da Venda"/>
     <tableColumn id="2" xr3:uid="{D98BEDD6-0C49-4F7A-8A6B-F1A8275F59BB}" name="Data"/>
     <tableColumn id="3" xr3:uid="{2497BEF2-F9CC-479D-944E-75AFB9C63334}" name="Produto"/>
-    <tableColumn id="4" xr3:uid="{95F6C9B9-35CA-45A8-BCB1-58B84AB19A5A}" name="Medida" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{95F6C9B9-35CA-45A8-BCB1-58B84AB19A5A}" name="Medida" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5910[[#This Row],[Produto]],cálculos!$M$7:$P$31,4,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{6BEBE7C6-A3F7-4015-B659-714498201054}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{A0018570-D78F-4AF7-863D-4A87B33FFEB6}" name="Preço Unitário" dataDxfId="4" dataCellStyle="Moeda">
+    <tableColumn id="6" xr3:uid="{A0018570-D78F-4AF7-863D-4A87B33FFEB6}" name="Preço Unitário" dataDxfId="6" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5910[[#This Row],[Produto]],cálculos!$M$7:$P$31,3,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{21D8DD35-CDAC-4A87-A570-E4AC6842F334}" name="SubTotal" dataDxfId="3" dataCellStyle="Moeda">
+    <tableColumn id="7" xr3:uid="{21D8DD35-CDAC-4A87-A570-E4AC6842F334}" name="SubTotal" dataDxfId="5" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela5910[[#This Row],[Preço Unitário]]*Tabela5910[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{45C60647-4AFD-46F9-BBCB-D010B8C4D5A3}" name="Desconto" dataCellStyle="Porcentagem"/>
     <tableColumn id="9" xr3:uid="{67B3CCC2-89B9-4DE5-8561-05A98ABA1597}" name="Entrega"/>
-    <tableColumn id="10" xr3:uid="{E679215B-C7A3-48DE-B602-5AE0FBCAAAE5}" name="Valor de Entrega" dataDxfId="2" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{E679215B-C7A3-48DE-B602-5AE0FBCAAAE5}" name="Valor de Entrega" dataDxfId="4" dataCellStyle="Moeda">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabela5910[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{043824D5-311C-4DEE-A15B-7E0406417187}" name="Total" dataDxfId="1" dataCellStyle="Moeda">
+    <tableColumn id="11" xr3:uid="{043824D5-311C-4DEE-A15B-7E0406417187}" name="Total" dataDxfId="3" dataCellStyle="Moeda">
       <calculatedColumnFormula>Tabela5910[[#This Row],[SubTotal]]*(1 - Tabela5910[[#This Row],[Desconto]])+Tabela5910[[#This Row],[Valor de Entrega]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{9F29B0E6-5B32-42BC-ABD3-C98CAF68E066}" name="Total para o Cliente" dataDxfId="0" dataCellStyle="Moeda">
+    <tableColumn id="12" xr3:uid="{9F29B0E6-5B32-42BC-ABD3-C98CAF68E066}" name="Total para o Cliente" dataDxfId="2" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela5910[[#This Row],[Id da Venda]]=B6,"",SUMIF(Tabela5910[Id da Venda],Tabela5910[[#This Row],[Id da Venda]],Tabela5910[Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4189,7 +5050,7 @@
   <dimension ref="B2:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:M19"/>
+      <selection activeCell="B5" sqref="B5:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4647,7 +5508,7 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="B5" sqref="B5:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5086,7 +5947,7 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7704,10 +8565,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H5:H28">
-    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="Atenção">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Atenção">
       <formula>NOT(ISERROR(SEARCH("Atenção",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="3" operator="containsText" text="Comprar">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Comprar">
       <formula>NOT(ISERROR(SEARCH("Comprar",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7758,13 +8619,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="20.7109375" customWidth="1"/>
@@ -7829,13 +8690,12 @@
     </row>
     <row r="10" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="31"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="37" t="s">
+      <c r="C10" s="37" t="s">
         <v>130</v>
       </c>
+      <c r="D10" s="37"/>
       <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38">
+      <c r="F10" s="38">
         <f>'Semana 1'!$M$31</f>
         <v>655.91200000000026</v>
       </c>
@@ -7850,13 +8710,12 @@
     </row>
     <row r="11" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="31"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="39" t="s">
+      <c r="C11" s="39" t="s">
         <v>131</v>
       </c>
+      <c r="D11" s="39"/>
       <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40">
+      <c r="F11" s="40">
         <f>'Semana 2'!M17</f>
         <v>103.82</v>
       </c>
@@ -7871,13 +8730,12 @@
     </row>
     <row r="12" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="31"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="39" t="s">
+      <c r="C12" s="39" t="s">
         <v>132</v>
       </c>
+      <c r="D12" s="39"/>
       <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40">
+      <c r="F12" s="40">
         <f>'Semana 3'!M17</f>
         <v>0</v>
       </c>
@@ -7892,13 +8750,12 @@
     </row>
     <row r="13" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="31"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="39" t="s">
+      <c r="C13" s="39" t="s">
         <v>133</v>
       </c>
+      <c r="D13" s="39"/>
       <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40">
+      <c r="F13" s="40">
         <f>'Semana 4'!M17</f>
         <v>0</v>
       </c>
@@ -7913,13 +8770,12 @@
     </row>
     <row r="14" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="31"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="41" t="s">
+      <c r="C14" s="41" t="s">
         <v>134</v>
       </c>
+      <c r="D14" s="41"/>
       <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42">
+      <c r="F14" s="42">
         <f>'Semana 5'!M17</f>
         <v>0</v>
       </c>
@@ -7934,11 +8790,10 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="31"/>
-      <c r="C15" s="27"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
       <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
@@ -7950,11 +8805,10 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="31"/>
-      <c r="C16" s="27"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
@@ -7966,15 +8820,14 @@
     </row>
     <row r="17" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="44" t="str">
+      <c r="C17" s="44" t="str">
         <f>"Total de vendas de "&amp;O5</f>
         <v>Total de vendas de Agosto</v>
       </c>
+      <c r="D17" s="44"/>
       <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45">
-        <f>SUM(G10:G14)</f>
+      <c r="F17" s="45">
+        <f>SUM(F10:F14)</f>
         <v>759.7320000000002</v>
       </c>
       <c r="H17" s="27"/>
@@ -8086,13 +8939,15 @@
     </row>
     <row r="26" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B26" s="31"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="37" t="s">
+      <c r="C26" s="37" t="s">
         <v>136</v>
       </c>
+      <c r="D26" s="37"/>
       <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
+      <c r="F26" s="47">
+        <f>SUM(COUNTIF(Tabela5[Valor de Entrega],"&gt;0"), COUNTIF(Tabela57[Valor de Entrega],"&gt;0"),COUNTIF(Tabela58[Valor de Entrega],"&gt;0"),COUNTIF(Tabela59[Valor de Entrega],"&gt;0"),COUNTIF(Tabela5910[Valor de Entrega],"&gt;0"),)/SUM('Semana 1'!M33,'Semana 2'!M19,'Semana 3'!M19,'Semana 4'!M19,'Semana 5'!M19)</f>
+        <v>0.5</v>
+      </c>
       <c r="H26" s="27"/>
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
@@ -8104,13 +8959,15 @@
     </row>
     <row r="27" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="31"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="39" t="s">
+      <c r="C27" s="39" t="s">
         <v>137</v>
       </c>
+      <c r="D27" s="39"/>
       <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="27"/>
+      <c r="F27" s="48">
+        <f>SUMIF(Tabela5[Valor de Entrega],"&gt;0",Tabela5[Total para o Cliente])+SUMIF(Tabela57[Valor de Entrega],"&gt;0",Tabela57[Total para o Cliente])+SUMIF(Tabela58[Valor de Entrega],"&gt;0",Tabela58[Total para o Cliente])+SUMIF(Tabela59[Valor de Entrega],"&gt;0",Tabela59[Total para o Cliente])+SUMIF(Tabela5910[Valor de Entrega],"&gt;0",Tabela5910[Total para o Cliente])</f>
+        <v>435.53200000000004</v>
+      </c>
       <c r="H27" s="27"/>
       <c r="I27" s="27"/>
       <c r="J27" s="27"/>
@@ -8122,13 +8979,12 @@
     </row>
     <row r="28" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="31"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="39" t="s">
+      <c r="C28" s="39" t="s">
         <v>138</v>
       </c>
+      <c r="D28" s="39"/>
       <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="40">
+      <c r="F28" s="40">
         <f>SUM('Semana 1'!M32,'Semana 2'!M18,'Semana 3'!M18,'Semana 4'!M18,'Semana 5'!M18)</f>
         <v>45.5</v>
       </c>
@@ -8147,7 +9003,6 @@
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
       <c r="H29" s="27"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
@@ -8163,7 +9018,6 @@
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
       <c r="H30" s="27"/>
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
@@ -8179,7 +9033,6 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
@@ -8195,7 +9048,6 @@
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
@@ -8211,7 +9063,6 @@
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27"/>
@@ -8223,13 +9074,15 @@
     </row>
     <row r="34" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="31"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="44" t="s">
+      <c r="C34" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="45"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="45">
+        <f>SUM('Semana 1'!M31,'Semana 2'!M17,'Semana 3'!M17,'Semana 4'!M17,'Semana 5'!M17)/SUM('Semana 1'!M33,'Semana 2'!M19,'Semana 3'!M19,'Semana 4'!M19,'Semana 5'!M19)</f>
+        <v>54.266571428571446</v>
+      </c>
+      <c r="F34" s="45"/>
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
       <c r="J34" s="27"/>
@@ -8300,7 +9153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C552C30-8CEE-4E95-8103-1820B67CA8FF}">
   <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33:M33"/>
     </sheetView>
   </sheetViews>
@@ -9495,7 +10348,7 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:M19"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aba Vendas (4 de 4) - Vendas por Região - Projeto
</commit_message>
<xml_diff>
--- a/Projeto/Projeto - Controle Mercado.xlsx
+++ b/Projeto/Projeto - Controle Mercado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zero\Desktop\Curso-Excel\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582CFDC9-11F1-4142-9944-866C9D18588C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6608CE-AD5E-41D1-B693-E1289E89EB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="141">
   <si>
     <t>Resultados</t>
   </si>
@@ -750,6 +750,9 @@
   </si>
   <si>
     <t>Número de Vendas</t>
+  </si>
+  <si>
+    <t>Quantidade de Venda por Região</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1064,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1121,6 +1124,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1333,19 +1338,367 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="7.5358705161854764E-2"/>
-          <c:y val="0.18300925925925926"/>
-          <c:w val="0.88853018372703407"/>
-          <c:h val="0.55283172936716241"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Vendas!$C$47:$C$51</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Loja</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Centro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zona Norte</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zona Oeste</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Zona Sul</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Vendas!$D$47:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6F36-4B3D-839F-E295319EBD70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1355,7 +1708,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1393,7 +1746,7 @@
                 <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1448,228 +1801,10 @@
             <c:numRef>
               <c:f>Vendas!$D$10:$D$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BD27-466B-93D5-B05232F480DA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Vendas!$C$10:$C$14</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Total de vendas semana 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total de vendas semana 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total de vendas semana 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total de vendas semana 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Total de vendas semana 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Vendas!$E$10:$E$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BD27-466B-93D5-B05232F480DA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Vendas!$C$10:$C$14</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Total de vendas semana 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total de vendas semana 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total de vendas semana 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total de vendas semana 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Total de vendas semana 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Vendas!$F$10:$F$14</c:f>
-              <c:numCache>
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>655.91200000000026</c:v>
+                  <c:v>662.41200000000026</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>103.82</c:v>
@@ -1688,12 +1823,12 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-BD27-466B-93D5-B05232F480DA}"/>
+              <c16:uniqueId val="{00000000-8953-4368-A551-F733B7B5826C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1703,11 +1838,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1951978415"/>
-        <c:axId val="1948964863"/>
+        <c:axId val="1894889391"/>
+        <c:axId val="1894884399"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1951978415"/>
+        <c:axId val="1894889391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,7 +1885,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1948964863"/>
+        <c:crossAx val="1894884399"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1758,7 +1893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1948964863"/>
+        <c:axId val="1894884399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,7 +1913,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1809,7 +1944,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1951978415"/>
+        <c:crossAx val="1894889391"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1837,12 +1972,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1865,17 +1995,17 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="106"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="6"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1917,8 +2047,8 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>
@@ -1931,7 +2061,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Vendas!$C$27:$C$28</c:f>
+              <c:f>Vendas!$C$28:$C$29</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1945,22 +2075,22 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Vendas!$F$27:$F$28</c:f>
+              <c:f>Vendas!$D$28:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>435.53200000000004</c:v>
+                  <c:v>477.27200000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.5</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2CE4-478E-A46D-CC810218A7C4}"/>
+              <c16:uniqueId val="{00000000-F8C9-4FC8-9BF1-DDB98DE47333}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1973,127 +2103,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="1002969151"/>
-        <c:axId val="1002967487"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent6"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Vendas!$C$27:$C$28</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>Vendas por Entrega (R$)</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Receita de Entregas (R$)</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Vendas!$D$27:$D$28</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-2CE4-478E-A46D-CC810218A7C4}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent5"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Vendas!$C$27:$C$28</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>Vendas por Entrega (R$)</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Receita de Entregas (R$)</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Vendas!$E$27:$E$28</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-2CE4-478E-A46D-CC810218A7C4}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-          </c:ext>
-        </c:extLst>
+        <c:axId val="1902260543"/>
+        <c:axId val="1902260959"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1002969151"/>
+        <c:axId val="1902260543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2136,7 +2150,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1002967487"/>
+        <c:crossAx val="1902260959"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2144,7 +2158,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1002967487"/>
+        <c:axId val="1902260959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2195,7 +2209,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1002969151"/>
+        <c:crossAx val="1902260543"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2209,6 +2223,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2216,12 +2237,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2245,10 +2261,13 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -2282,43 +2301,537 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
-  <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
   <a:schemeClr val="accent4"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2821,7 +3334,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4158,14 +4671,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
@@ -4183,8 +4696,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8420100" y="171450"/>
-          <a:ext cx="1352550" cy="419100"/>
+          <a:off x="9791700" y="171450"/>
+          <a:ext cx="2124075" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4220,23 +4733,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2">
+        <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8BFE13B-9D84-43FC-94C9-01C34B3F6438}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71509F58-8380-4D1D-B946-79306E43BC2F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4256,23 +4769,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>80961</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Gráfico 6">
+        <xdr:cNvPr id="9" name="Gráfico 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D927DE6-C913-4396-800C-254D05373E1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D075FAA-4CD2-43B4-A5DC-20A00B380F52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4285,6 +4798,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46535C78-170E-451B-8B54-6EA80B712E68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5005,7 +5554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:B13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5947,7 +6496,7 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6385,7 +6934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B6:P30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -8617,34 +9166,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B1:O38"/>
+  <dimension ref="B1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:15" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:19" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:15" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="O5" s="36" t="s">
+    <row r="3" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M5" s="36"/>
+      <c r="N5" s="36" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" s="28"/>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -8657,10 +9208,9 @@
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="30"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="30"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="31"/>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
@@ -8673,10 +9223,10 @@
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="32"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="32"/>
+      <c r="R8" s="27"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="31"/>
       <c r="C9" s="27"/>
       <c r="H9" s="27"/>
@@ -8685,19 +9235,17 @@
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
       <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="32"/>
-    </row>
-    <row r="10" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N9" s="32"/>
+      <c r="R9" s="27"/>
+    </row>
+    <row r="10" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="31"/>
       <c r="C10" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38">
+      <c r="D10" s="38">
         <f>'Semana 1'!$M$31</f>
-        <v>655.91200000000026</v>
+        <v>662.41200000000026</v>
       </c>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
@@ -8705,17 +9253,15 @@
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
       <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="32"/>
-    </row>
-    <row r="11" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N10" s="32"/>
+      <c r="R10" s="27"/>
+    </row>
+    <row r="11" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="31"/>
       <c r="C11" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40">
+      <c r="D11" s="40">
         <f>'Semana 2'!M17</f>
         <v>103.82</v>
       </c>
@@ -8725,17 +9271,15 @@
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="32"/>
-    </row>
-    <row r="12" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N11" s="32"/>
+      <c r="R11" s="27"/>
+    </row>
+    <row r="12" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="31"/>
       <c r="C12" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40">
+      <c r="D12" s="40">
         <f>'Semana 3'!M17</f>
         <v>0</v>
       </c>
@@ -8745,17 +9289,15 @@
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="32"/>
-    </row>
-    <row r="13" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N12" s="32"/>
+      <c r="R12" s="27"/>
+    </row>
+    <row r="13" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="31"/>
       <c r="C13" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40">
+      <c r="D13" s="40">
         <f>'Semana 4'!M17</f>
         <v>0</v>
       </c>
@@ -8765,17 +9307,15 @@
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="32"/>
-    </row>
-    <row r="14" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N13" s="32"/>
+      <c r="R13" s="27"/>
+    </row>
+    <row r="14" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="31"/>
       <c r="C14" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42">
+      <c r="D14" s="42">
         <f>'Semana 5'!M17</f>
         <v>0</v>
       </c>
@@ -8785,50 +9325,45 @@
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="32"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="32"/>
+      <c r="R14" s="27"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="31"/>
       <c r="C15" s="43"/>
       <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="32"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="32"/>
+      <c r="R15" s="27"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="31"/>
       <c r="C16" s="43"/>
       <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
       <c r="K16" s="27"/>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="32"/>
-    </row>
-    <row r="17" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N16" s="32"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+    </row>
+    <row r="17" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
       <c r="C17" s="44" t="str">
-        <f>"Total de vendas de "&amp;O5</f>
+        <f>"Total de vendas de "&amp;N5</f>
         <v>Total de vendas de Agosto</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="45">
-        <f>SUM(F10:F14)</f>
-        <v>759.7320000000002</v>
+      <c r="D17" s="45">
+        <f>SUM(D10:D14)</f>
+        <v>766.2320000000002</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="27"/>
@@ -8836,10 +9371,11 @@
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="32"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N17" s="32"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="31"/>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
@@ -8852,10 +9388,11 @@
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="32"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N18" s="32"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="31"/>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
@@ -8868,10 +9405,11 @@
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="32"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N19" s="32"/>
+      <c r="R19" s="27"/>
+      <c r="S19" s="27"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="31"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
@@ -8884,10 +9422,11 @@
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="32"/>
-    </row>
-    <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="32"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+    </row>
+    <row r="21" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="33"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
@@ -8900,12 +9439,18 @@
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="35"/>
-    </row>
-    <row r="22" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="35"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+    </row>
+    <row r="22" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+    </row>
+    <row r="23" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S23" s="27"/>
+    </row>
+    <row r="24" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
@@ -8918,10 +9463,10 @@
       <c r="K24" s="29"/>
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="30"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N24" s="30"/>
+      <c r="S24" s="27"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="31"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
@@ -8934,39 +9479,28 @@
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="32"/>
-    </row>
-    <row r="26" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N25" s="32"/>
+      <c r="S25" s="27"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="31"/>
-      <c r="C26" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="47">
-        <f>SUM(COUNTIF(Tabela5[Valor de Entrega],"&gt;0"), COUNTIF(Tabela57[Valor de Entrega],"&gt;0"),COUNTIF(Tabela58[Valor de Entrega],"&gt;0"),COUNTIF(Tabela59[Valor de Entrega],"&gt;0"),COUNTIF(Tabela5910[Valor de Entrega],"&gt;0"),)/SUM('Semana 1'!M33,'Semana 2'!M19,'Semana 3'!M19,'Semana 4'!M19,'Semana 5'!M19)</f>
-        <v>0.5</v>
-      </c>
       <c r="H26" s="27"/>
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="32"/>
-    </row>
-    <row r="27" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N26" s="32"/>
+      <c r="S26" s="27"/>
+    </row>
+    <row r="27" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="31"/>
-      <c r="C27" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="48">
-        <f>SUMIF(Tabela5[Valor de Entrega],"&gt;0",Tabela5[Total para o Cliente])+SUMIF(Tabela57[Valor de Entrega],"&gt;0",Tabela57[Total para o Cliente])+SUMIF(Tabela58[Valor de Entrega],"&gt;0",Tabela58[Total para o Cliente])+SUMIF(Tabela59[Valor de Entrega],"&gt;0",Tabela59[Total para o Cliente])+SUMIF(Tabela5910[Valor de Entrega],"&gt;0",Tabela5910[Total para o Cliente])</f>
-        <v>435.53200000000004</v>
+      <c r="C27" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="47">
+        <f>SUM(COUNTIF(Tabela5[Valor de Entrega],"&gt;0"), COUNTIF(Tabela57[Valor de Entrega],"&gt;0"),COUNTIF(Tabela58[Valor de Entrega],"&gt;0"),COUNTIF(Tabela59[Valor de Entrega],"&gt;0"),COUNTIF(Tabela5910[Valor de Entrega],"&gt;0"),)/SUM('Semana 1'!M33,'Semana 2'!M19,'Semana 3'!M19,'Semana 4'!M19,'Semana 5'!M19)</f>
+        <v>0.5714285714285714</v>
       </c>
       <c r="H27" s="27"/>
       <c r="I27" s="27"/>
@@ -8974,19 +9508,17 @@
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
       <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="32"/>
-    </row>
-    <row r="28" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N27" s="32"/>
+      <c r="S27" s="27"/>
+    </row>
+    <row r="28" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="31"/>
       <c r="C28" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40">
-        <f>SUM('Semana 1'!M32,'Semana 2'!M18,'Semana 3'!M18,'Semana 4'!M18,'Semana 5'!M18)</f>
-        <v>45.5</v>
+        <v>137</v>
+      </c>
+      <c r="D28" s="48">
+        <f>SUMIF(Tabela5[Valor de Entrega],"&gt;0",Tabela5[Total para o Cliente])+SUMIF(Tabela57[Valor de Entrega],"&gt;0",Tabela57[Total para o Cliente])+SUMIF(Tabela58[Valor de Entrega],"&gt;0",Tabela58[Total para o Cliente])+SUMIF(Tabela59[Valor de Entrega],"&gt;0",Tabela59[Total para o Cliente])+SUMIF(Tabela5910[Valor de Entrega],"&gt;0",Tabela5910[Total para o Cliente])</f>
+        <v>477.27200000000005</v>
       </c>
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
@@ -8994,25 +9526,29 @@
       <c r="K28" s="27"/>
       <c r="L28" s="27"/>
       <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="32"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N28" s="32"/>
+      <c r="S28" s="27"/>
+    </row>
+    <row r="29" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B29" s="31"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
+      <c r="C29" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="40">
+        <f>SUM('Semana 1'!M32,'Semana 2'!M18,'Semana 3'!M18,'Semana 4'!M18,'Semana 5'!M18)</f>
+        <v>52</v>
+      </c>
       <c r="H29" s="27"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
       <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="32"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N29" s="32"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="31"/>
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
@@ -9024,10 +9560,10 @@
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="32"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N30" s="32"/>
+      <c r="T30" s="27"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="31"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
@@ -9039,10 +9575,10 @@
       <c r="K31" s="27"/>
       <c r="L31" s="27"/>
       <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="32"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N31" s="32"/>
+      <c r="T31" s="27"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="31"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
@@ -9054,10 +9590,10 @@
       <c r="K32" s="27"/>
       <c r="L32" s="27"/>
       <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="32"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N32" s="32"/>
+      <c r="T32" s="27"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="31"/>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
@@ -9069,18 +9605,17 @@
       <c r="K33" s="27"/>
       <c r="L33" s="27"/>
       <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="32"/>
-    </row>
-    <row r="34" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N33" s="32"/>
+      <c r="T33" s="27"/>
+    </row>
+    <row r="34" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="31"/>
       <c r="C34" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="44"/>
-      <c r="E34" s="45">
+      <c r="D34" s="45">
         <f>SUM('Semana 1'!M31,'Semana 2'!M17,'Semana 3'!M17,'Semana 4'!M17,'Semana 5'!M17)/SUM('Semana 1'!M33,'Semana 2'!M19,'Semana 3'!M19,'Semana 4'!M19,'Semana 5'!M19)</f>
-        <v>54.266571428571446</v>
+        <v>54.730857142857154</v>
       </c>
       <c r="F34" s="45"/>
       <c r="H34" s="27"/>
@@ -9089,10 +9624,10 @@
       <c r="K34" s="27"/>
       <c r="L34" s="27"/>
       <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="32"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N34" s="32"/>
+      <c r="T34" s="27"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="31"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
@@ -9105,10 +9640,10 @@
       <c r="K35" s="27"/>
       <c r="L35" s="27"/>
       <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="32"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N35" s="32"/>
+      <c r="T35" s="27"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="31"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
@@ -9121,10 +9656,10 @@
       <c r="K36" s="27"/>
       <c r="L36" s="27"/>
       <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="32"/>
-    </row>
-    <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N36" s="32"/>
+      <c r="T36" s="27"/>
+    </row>
+    <row r="37" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="33"/>
       <c r="C37" s="34"/>
       <c r="D37" s="34"/>
@@ -9137,10 +9672,254 @@
       <c r="K37" s="34"/>
       <c r="L37" s="34"/>
       <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="35"/>
-    </row>
-    <row r="38" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="N37" s="35"/>
+      <c r="T37" s="27"/>
+    </row>
+    <row r="38" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="T38" s="27"/>
+    </row>
+    <row r="39" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T39" s="27"/>
+    </row>
+    <row r="40" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="28"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="30"/>
+      <c r="T40" s="27"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="31"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="32"/>
+      <c r="T41" s="27"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="31"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="32"/>
+      <c r="T42" s="27"/>
+    </row>
+    <row r="43" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B43" s="31"/>
+      <c r="C43" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="32"/>
+      <c r="T43" s="27"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="31"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+      <c r="N44" s="32"/>
+      <c r="T44" s="27"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="31"/>
+      <c r="E45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="32"/>
+      <c r="T45" s="27"/>
+    </row>
+    <row r="46" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B46" s="31"/>
+      <c r="D46" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" s="50"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="32"/>
+      <c r="T46" s="27"/>
+    </row>
+    <row r="47" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B47" s="31"/>
+      <c r="C47" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="37">
+        <f>COUNTIFS(Tabela5[Entrega],Vendas!C47,Tabela5[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela57[Entrega],Vendas!C47,Tabela57[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela58[Entrega],Vendas!C47,Tabela58[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela59[Entrega],Vendas!C47,Tabela59[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela5910[Entrega],Vendas!C47,Tabela5910[Total para o Cliente],"&gt;0")</f>
+        <v>6</v>
+      </c>
+      <c r="E47" s="50"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="27"/>
+      <c r="N47" s="32"/>
+      <c r="T47" s="27"/>
+    </row>
+    <row r="48" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B48" s="31"/>
+      <c r="C48" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" s="37">
+        <f>COUNTIFS(Tabela5[Entrega],Vendas!C48,Tabela5[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela57[Entrega],Vendas!C48,Tabela57[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela58[Entrega],Vendas!C48,Tabela58[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela59[Entrega],Vendas!C48,Tabela59[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela5910[Entrega],Vendas!C48,Tabela5910[Total para o Cliente],"&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="E48" s="50"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+      <c r="N48" s="32"/>
+      <c r="T48" s="27"/>
+    </row>
+    <row r="49" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B49" s="31"/>
+      <c r="C49" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="37">
+        <f>COUNTIFS(Tabela5[Entrega],Vendas!C49,Tabela5[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela57[Entrega],Vendas!C49,Tabela57[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela58[Entrega],Vendas!C49,Tabela58[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela59[Entrega],Vendas!C49,Tabela59[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela5910[Entrega],Vendas!C49,Tabela5910[Total para o Cliente],"&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="E49" s="50"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="27"/>
+      <c r="N49" s="32"/>
+      <c r="T49" s="27"/>
+    </row>
+    <row r="50" spans="2:20" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B50" s="31"/>
+      <c r="C50" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="37">
+        <f>COUNTIFS(Tabela5[Entrega],Vendas!C50,Tabela5[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela57[Entrega],Vendas!C50,Tabela57[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela58[Entrega],Vendas!C50,Tabela58[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela59[Entrega],Vendas!C50,Tabela59[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela5910[Entrega],Vendas!C50,Tabela5910[Total para o Cliente],"&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="E50" s="50"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="27"/>
+      <c r="N50" s="32"/>
+    </row>
+    <row r="51" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B51" s="31"/>
+      <c r="C51" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="37">
+        <f>COUNTIFS(Tabela5[Entrega],Vendas!C51,Tabela5[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela57[Entrega],Vendas!C51,Tabela57[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela58[Entrega],Vendas!C51,Tabela58[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela59[Entrega],Vendas!C51,Tabela59[Total para o Cliente],"&gt;0")+COUNTIFS(Tabela5910[Entrega],Vendas!C51,Tabela5910[Total para o Cliente],"&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="E51" s="50"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="27"/>
+      <c r="N51" s="32"/>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="31"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="27"/>
+      <c r="N52" s="32"/>
+    </row>
+    <row r="53" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="34"/>
+      <c r="N53" s="35"/>
+    </row>
+    <row r="54" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -9153,8 +9932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C552C30-8CEE-4E95-8103-1820B67CA8FF}">
   <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:M33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9501,7 +10280,7 @@
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K11" s="4">
         <f>IF(Tabela5[[#This Row],[Id da Venda]]=B12,0,VLOOKUP(Tabela5[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE))</f>
@@ -9543,19 +10322,19 @@
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K12" s="4">
         <f>IF(Tabela5[[#This Row],[Id da Venda]]=B13,0,VLOOKUP(Tabela5[[#This Row],[Entrega]],cálculos!$B$7:$C$11,2,FALSE))</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="L12" s="4">
         <f>Tabela5[[#This Row],[SubTotal]]*(1 - Tabela5[[#This Row],[Desconto]])+Tabela5[[#This Row],[Valor de Entrega]]</f>
-        <v>9.56</v>
+        <v>16.060000000000002</v>
       </c>
       <c r="M12" s="4">
         <f>IF(Tabela5[[#This Row],[Id da Venda]]=B13,"",SUMIF(Tabela5[Id da Venda],Tabela5[[#This Row],[Id da Venda]],Tabela5[Total]))</f>
-        <v>35.24</v>
+        <v>41.74</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -10292,7 +11071,7 @@
       <c r="L31" s="21"/>
       <c r="M31" s="21">
         <f>SUM(Tabela5[Total])</f>
-        <v>655.91200000000026</v>
+        <v>662.41200000000026</v>
       </c>
     </row>
     <row r="32" spans="2:13" ht="21" x14ac:dyDescent="0.35">
@@ -10311,7 +11090,7 @@
       <c r="L32" s="23"/>
       <c r="M32" s="23">
         <f>SUM(Tabela5[Valor de Entrega])</f>
-        <v>40.5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:13" ht="21" x14ac:dyDescent="0.35">
@@ -10340,6 +11119,18 @@
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D98FB369-EF8B-460C-AEB6-76CF3DDC68A8}">
+          <x14:formula1>
+            <xm:f>cálculos!$B$7:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>J5:J29</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10348,7 +11139,7 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10763,7 +11554,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C0AF14DC-739D-4BB4-BAAA-60C26B752615}">
           <x14:formula1>
             <xm:f>cálculos!$B$7:$B$11</xm:f>

</xml_diff>